<commit_message>
complete deep search result
</commit_message>
<xml_diff>
--- a/model/data.xlsx
+++ b/model/data.xlsx
@@ -1416,7 +1416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
@@ -1923,9 +1923,79 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="14.4" customHeight="1"/>
-    <row r="19" ht="14.4" customHeight="1"/>
-    <row r="20" ht="14.4" customHeight="1"/>
+    <row r="18" ht="14.4" customHeight="1">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>x2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="14.4" customHeight="1">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>x3</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" t="n">
+        <v>28</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="G19" t="n">
+        <v>20000000</v>
+      </c>
+      <c r="H19" t="n">
+        <v>3000000000</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Quận 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="14.4" customHeight="1">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>x4</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" t="n">
+        <v>30</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" t="n">
+        <v>42000000</v>
+      </c>
+      <c r="G20" t="n">
+        <v>25000000</v>
+      </c>
+      <c r="H20" t="n">
+        <v>3500000000</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Quận 9</t>
+        </is>
+      </c>
+    </row>
     <row r="21" ht="14.4" customHeight="1"/>
     <row r="22" ht="14.4" customHeight="1"/>
     <row r="23" ht="14.4" customHeight="1"/>
@@ -30266,7 +30336,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
@@ -30338,20 +30408,116 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>test121@</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0987654321</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Bình Tân, Tp. Hồ Chí Minh</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>69669639af0907575e18.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>x2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>user4989</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>test@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>test@123</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>x3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Phan Nghĩa</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>phannghia@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>phannghia@123</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0562612494</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Bình Tân, Tp. Hồ Chí Minh</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Goku-Ultra-Instinct-PC-Wallpaper.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>x4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Nguyen Van A</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>phannghia1@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>phannghia1@</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>0987654321</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Bình Tân, Tp. Hồ Chí Minh</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>b80c48ae0334e8499458332def163dba-1068x601.jpg</t>
         </is>

</xml_diff>

<commit_message>
update Loan Comparison function
</commit_message>
<xml_diff>
--- a/model/data.xlsx
+++ b/model/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="658" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="rules" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,10 +22,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -105,14 +106,6 @@
       <sz val="12"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -122,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -145,13 +138,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
@@ -167,9 +173,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -242,9 +259,45 @@
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="7"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="8"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="8">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="9">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="7"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="10">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="10">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="10">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="10">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="11">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="11">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="9">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Comma 2" xfId="2"/>
@@ -253,7 +306,10 @@
     <cellStyle name="Normal 5" xfId="5"/>
     <cellStyle name="Normal 6" xfId="6"/>
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
+    <cellStyle name="Normal 7" xfId="8"/>
+    <cellStyle name="Comma 3" xfId="9"/>
+    <cellStyle name="Normal 8" xfId="10"/>
+    <cellStyle name="Normal 9" xfId="11"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -630,15 +686,15 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
   <cols>
     <col width="13.33203125" customWidth="1" min="1" max="1"/>
     <col width="12.88671875" customWidth="1" min="2" max="2"/>
-    <col width="49.88671875" customWidth="1" min="4" max="4"/>
+    <col width="49.88671875" customWidth="1" style="39" min="4" max="4"/>
     <col width="55.44140625" customWidth="1" min="5" max="5"/>
     <col width="74" customWidth="1" min="6" max="6"/>
   </cols>
@@ -659,7 +715,7 @@
           <t>score</t>
         </is>
       </c>
-      <c r="D1" s="15" t="inlineStr">
+      <c r="D1" s="35" t="inlineStr">
         <is>
           <t>rule_expression</t>
         </is>
@@ -689,7 +745,7 @@
       <c r="C2" s="16" t="n">
         <v>0.7</v>
       </c>
-      <c r="D2" s="16" t="inlineStr">
+      <c r="D2" s="36" t="inlineStr">
         <is>
           <t>(getValue(buyerInfo.get("group",  0))  == 1 or (buyerInfo.get("is_married")  == False and buyerInfo.get("no_child") == 0 )) and houseInfo.get("in_room_noBed")  in (1, 2)</t>
         </is>
@@ -719,7 +775,7 @@
       <c r="C3" s="16" t="n">
         <v>0.6</v>
       </c>
-      <c r="D3" s="16" t="inlineStr">
+      <c r="D3" s="36" t="inlineStr">
         <is>
           <t>(getValue(buyerInfo.get("group",  0))  == 1 or (buyerInfo.get("is_married")  == False and buyerInfo.get("no_child") == 0 )) and houseInfo.get("in_room_noBed")  in (2,3,4)</t>
         </is>
@@ -749,7 +805,7 @@
       <c r="C4" s="16" t="n">
         <v>0.8</v>
       </c>
-      <c r="D4" s="16" t="inlineStr">
+      <c r="D4" s="36" t="inlineStr">
         <is>
           <t>( getValue(buyerInfo.get("group",  0))  == 2 or buyerInfo.get("is_married")  == True ) and buyerInfo.get("no_child") in ( 0, 1) and houseInfo.get("in_room_noBed")  in (2, 3,4)</t>
         </is>
@@ -779,7 +835,7 @@
       <c r="C5" s="16" t="n">
         <v>0.6</v>
       </c>
-      <c r="D5" s="16" t="inlineStr">
+      <c r="D5" s="36" t="inlineStr">
         <is>
           <t>( getValue(buyerInfo.get("group",  0))  == 2 or buyerInfo.get("is_married")  == True ) and buyerInfo.get("no_child") in ( 0, 1) and houseInfo.get("in_room_noBed")  == 1</t>
         </is>
@@ -809,7 +865,7 @@
       <c r="C6" s="16" t="n">
         <v>0.5</v>
       </c>
-      <c r="D6" s="16" t="inlineStr">
+      <c r="D6" s="36" t="inlineStr">
         <is>
           <t>( getValue(buyerInfo.get("group",  0))  == 2 or buyerInfo.get("is_married")  == True ) and buyerInfo.get("no_child") == 2 and houseInfo.get("in_room_noBed")  == 2</t>
         </is>
@@ -839,7 +895,7 @@
       <c r="C7" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="16" t="inlineStr">
+      <c r="D7" s="36" t="inlineStr">
         <is>
           <t>( getValue(buyerInfo.get("group",  0))  == 2 or buyerInfo.get("is_married")  == True )  and buyerInfo.get("no_child") == 2 and houseInfo.get("in_room_noBed")  in ( 3,4,5)</t>
         </is>
@@ -869,7 +925,7 @@
       <c r="C8" s="16" t="n">
         <v>0.6</v>
       </c>
-      <c r="D8" s="16" t="inlineStr">
+      <c r="D8" s="36" t="inlineStr">
         <is>
           <t>getValue(buyerInfo.get("group",  0))  == 4 and houseInfo.get("in_room_noBed")  == 1</t>
         </is>
@@ -899,7 +955,7 @@
       <c r="C9" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="16" t="inlineStr">
+      <c r="D9" s="36" t="inlineStr">
         <is>
           <t>getValue(buyerInfo.get("group",  0))  == 4 and houseInfo.get("in_room_noBed")  in (2, 3,4)</t>
         </is>
@@ -929,7 +985,7 @@
       <c r="C10" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="17" t="inlineStr">
+      <c r="D10" s="37" t="inlineStr">
         <is>
           <t>houseInfo.get("price") &gt;= 0.9 * buyerInfo.get("avai_amt") and houseInfo.get("price") &lt;= buyerInfo.get("avai_amt")</t>
         </is>
@@ -959,7 +1015,7 @@
       <c r="C11" s="18" t="n">
         <v>0.8</v>
       </c>
-      <c r="D11" s="19" t="inlineStr">
+      <c r="D11" s="38" t="inlineStr">
         <is>
           <t>( buyerInfo.get("avai_amt")  &gt;= 0.75 * houseInfo.get("price") and houseInfo.get("price") &gt; buyerInfo.get("avai_amt") ) and ( (buyerInfo.get("avai_amt") + 12* buyerInfo.get("monthly_amt")) &gt;= houseInfo.get("price"))</t>
         </is>
@@ -985,7 +1041,7 @@
       <c r="C12" s="18" t="n">
         <v>0.6</v>
       </c>
-      <c r="D12" s="19" t="inlineStr">
+      <c r="D12" s="38" t="inlineStr">
         <is>
           <t>( buyerInfo.get("avai_amt")  &gt;= 0.5 * houseInfo.get("price") and houseInfo.get("price") &gt; buyerInfo.get("avai_amt") ) and ( (buyerInfo.get("avai_amt") + 24* buyerInfo.get("monthly_amt")) &gt;= houseInfo.get("price"))</t>
         </is>
@@ -1015,7 +1071,7 @@
       <c r="C13" s="18" t="n">
         <v>0.5</v>
       </c>
-      <c r="D13" s="19" t="inlineStr">
+      <c r="D13" s="38" t="inlineStr">
         <is>
           <t>( buyerInfo.get("avai_amt")  &gt;= 0.5 * houseInfo.get("price") and houseInfo.get("price") &gt; buyerInfo.get("avai_amt") ) and ( (buyerInfo.get("avai_amt") + 60* buyerInfo.get("monthly_amt")) &gt;= houseInfo.get("price"))</t>
         </is>
@@ -1041,7 +1097,7 @@
       <c r="C14" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D14" s="19" t="inlineStr">
+      <c r="D14" s="38" t="inlineStr">
         <is>
           <t>getValue(buyerInfo.get("group",  0))  == 4 and ( houseInfo.get("price") &gt;= 0.8 * buyerInfo.get("avai_amt") and houseInfo.get("price") &lt;= buyerInfo.get("avai_amt")*1.2 )</t>
         </is>
@@ -1067,7 +1123,7 @@
       <c r="C15" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="D15" s="19" t="inlineStr">
+      <c r="D15" s="38" t="inlineStr">
         <is>
           <t>getValue(buyerInfo.get("group",  0))  == 4 and ( houseInfo.get("price") &lt; 0.8 * buyerInfo.get("avai_amt") and houseInfo.get("price") &gt; buyerInfo.get("avai_amt")*1.2 )</t>
         </is>
@@ -1093,7 +1149,7 @@
       <c r="C16" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="19" t="inlineStr">
+      <c r="D16" s="38" t="inlineStr">
         <is>
           <t>fn_calculateDistance(houseInfo.get("address_district"), buyerInfo.get("desired_location")) &lt;= 2</t>
         </is>
@@ -1119,7 +1175,7 @@
       <c r="C17" s="21" t="n">
         <v>0.8</v>
       </c>
-      <c r="D17" s="19" t="inlineStr">
+      <c r="D17" s="38" t="inlineStr">
         <is>
           <t>fn_calculateDistance(houseInfo.get("address_district"), buyerInfo.get("desired_location")) &lt;= 4</t>
         </is>
@@ -1141,7 +1197,7 @@
       <c r="C18" s="21" t="n">
         <v>0.5</v>
       </c>
-      <c r="D18" s="19" t="inlineStr">
+      <c r="D18" s="38" t="inlineStr">
         <is>
           <t>fn_calculateDistance(houseInfo.get("address_district"), buyerInfo.get("desired_location")) &lt;= 6</t>
         </is>
@@ -1163,7 +1219,7 @@
       <c r="C19" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="19" t="inlineStr">
+      <c r="D19" s="38" t="inlineStr">
         <is>
           <t>isGoodLegalStatus(houseInfo.get("legal_status"))</t>
         </is>
@@ -1193,7 +1249,7 @@
       <c r="C20" s="21" t="n">
         <v>0.2</v>
       </c>
-      <c r="D20" s="19" t="inlineStr">
+      <c r="D20" s="38" t="inlineStr">
         <is>
           <t>isGoodLegalStatus(houseInfo.get("legal_status")) is not True and getValue(buyerInfo.get("group",  0)) in (1, 3,4)</t>
         </is>
@@ -1219,7 +1275,7 @@
       <c r="C21" s="21" t="n">
         <v>0.4</v>
       </c>
-      <c r="D21" s="19" t="inlineStr">
+      <c r="D21" s="38" t="inlineStr">
         <is>
           <t>isGoodLegalStatus(houseInfo.get("legal_status")) is not True and getValue(buyerInfo.get("group",  0)) not in (1, 3,4)</t>
         </is>
@@ -1245,7 +1301,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1265,7 +1321,7 @@
           <t>rule_group</t>
         </is>
       </c>
-      <c r="B1" s="12" t="inlineStr">
+      <c r="B1" s="40" t="inlineStr">
         <is>
           <t>conditions</t>
         </is>
@@ -1298,9 +1354,9 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B2" s="12" t="inlineStr">
-        <is>
-          <t>isValidInput(buyerInfo.get("group")) and isValidInput( buyerInfo.get("is_married")) and isValidInput( buyerInfo.get("no_child")) and isValidInput(houseInfo.get("in_room_noBed"))</t>
+      <c r="B2" s="40" t="inlineStr">
+        <is>
+          <t>isValidInput( buyerInfo.get("group") )  and isValidInput( buyerInfo.get("is_married") )  and isValidInput( buyerInfo.get("no_child") )  and isValidInput(houseInfo.get("no_bedroom") )</t>
         </is>
       </c>
       <c r="C2" s="12" t="n"/>
@@ -1329,9 +1385,9 @@
           <t>B</t>
         </is>
       </c>
-      <c r="B3" s="12" t="inlineStr">
-        <is>
-          <t>isNotNoneInput(buyerInfo.get("avai_amt")) and isNotNoneInput(buyerInfo.get("monthly_amt"))</t>
+      <c r="B3" s="40" t="inlineStr">
+        <is>
+          <t>buyerInfo.get("avai_amt") is not None and buyerInfo.get("monthly_amt") is not None</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -1360,7 +1416,7 @@
           <t>C</t>
         </is>
       </c>
-      <c r="B4" s="14" t="inlineStr">
+      <c r="B4" s="41" t="inlineStr">
         <is>
           <t xml:space="preserve">isValidInput( buyerInfo.get("desired_location") ) and isValidInput( houseInfo.get("address_district") ) </t>
         </is>
@@ -1391,7 +1447,7 @@
           <t>D</t>
         </is>
       </c>
-      <c r="B5" s="14" t="inlineStr">
+      <c r="B5" s="41" t="inlineStr">
         <is>
           <t>1==1</t>
         </is>
@@ -1427,26 +1483,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J19" sqref="A17:J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col width="3.5546875" bestFit="1" customWidth="1" style="22" min="1" max="1"/>
-    <col width="7.33203125" customWidth="1" style="22" min="2" max="2"/>
-    <col width="8.88671875" customWidth="1" style="22" min="3" max="3"/>
-    <col width="11.33203125" bestFit="1" customWidth="1" style="22" min="4" max="4"/>
-    <col width="9.6640625" customWidth="1" style="22" min="5" max="5"/>
+    <col width="3.5546875" bestFit="1" customWidth="1" style="43" min="1" max="1"/>
+    <col width="7.33203125" customWidth="1" style="43" min="2" max="2"/>
+    <col width="8.88671875" customWidth="1" style="43" min="3" max="3"/>
+    <col width="11.33203125" bestFit="1" customWidth="1" style="43" min="4" max="4"/>
+    <col width="9.6640625" customWidth="1" style="43" min="5" max="5"/>
     <col width="15.33203125" customWidth="1" style="28" min="6" max="6"/>
     <col width="15.77734375" customWidth="1" style="28" min="7" max="7"/>
     <col width="18.109375" bestFit="1" customWidth="1" style="28" min="8" max="8"/>
-    <col width="18.21875" customWidth="1" style="22" min="9" max="9"/>
-    <col width="22.88671875" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
-    <col width="8.88671875" customWidth="1" style="22" min="11" max="42"/>
-    <col width="8.88671875" customWidth="1" style="22" min="43" max="16384"/>
+    <col width="18.21875" customWidth="1" style="43" min="9" max="9"/>
+    <col width="22.88671875" bestFit="1" customWidth="1" style="43" min="10" max="10"/>
+    <col width="8.88671875" customWidth="1" style="43" min="11" max="43"/>
+    <col width="8.88671875" customWidth="1" style="43" min="44" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1500,7 +1556,7 @@
           <t>desired_interiorStatus</t>
         </is>
       </c>
-      <c r="K1" s="8" t="n"/>
+      <c r="K1" s="42" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
@@ -1535,7 +1591,7 @@
         </is>
       </c>
       <c r="J2" s="7" t="n"/>
-      <c r="K2" s="8" t="n"/>
+      <c r="K2" s="42" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
@@ -1570,7 +1626,7 @@
         </is>
       </c>
       <c r="J3" s="7" t="n"/>
-      <c r="K3" s="8" t="n"/>
+      <c r="K3" s="42" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
@@ -1605,7 +1661,7 @@
         </is>
       </c>
       <c r="J4" s="7" t="n"/>
-      <c r="K4" s="8" t="n"/>
+      <c r="K4" s="42" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
@@ -1640,7 +1696,7 @@
         </is>
       </c>
       <c r="J5" s="7" t="n"/>
-      <c r="K5" s="8" t="n"/>
+      <c r="K5" s="42" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
@@ -1665,7 +1721,7 @@
       <c r="H6" s="26" t="n"/>
       <c r="I6" s="7" t="n"/>
       <c r="J6" s="7" t="n"/>
-      <c r="K6" s="8" t="n"/>
+      <c r="K6" s="42" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
@@ -1680,7 +1736,7 @@
         <v>30</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>2</v>
@@ -1859,7 +1915,7 @@
         </is>
       </c>
       <c r="J14" s="7" t="n"/>
-      <c r="K14" s="8" t="n"/>
+      <c r="K14" s="42" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="7" t="inlineStr">
@@ -1880,63 +1936,167 @@
         </is>
       </c>
       <c r="J15" s="7" t="n"/>
-      <c r="K15" s="8" t="n"/>
+      <c r="K15" s="42" t="n"/>
+      <c r="L15" s="43" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="inlineStr">
+      <c r="A16" s="33" t="inlineStr">
         <is>
           <t>D1</t>
         </is>
       </c>
-      <c r="B16" s="7" t="n">
+      <c r="B16" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="C16" s="7" t="n"/>
-      <c r="D16" s="7" t="n"/>
-      <c r="E16" s="7" t="n"/>
-      <c r="F16" s="26" t="n"/>
-      <c r="G16" s="26" t="n"/>
-      <c r="H16" s="26" t="n"/>
-      <c r="I16" s="7" t="n"/>
-      <c r="J16" s="7" t="n"/>
-      <c r="K16" s="8" t="n"/>
+      <c r="C16" s="33" t="n"/>
+      <c r="D16" s="33" t="n"/>
+      <c r="E16" s="33" t="n"/>
+      <c r="F16" s="34" t="n"/>
+      <c r="G16" s="34" t="n"/>
+      <c r="H16" s="34" t="n"/>
+      <c r="I16" s="33" t="n"/>
+      <c r="J16" s="33" t="n"/>
+      <c r="K16" s="42" t="n"/>
+      <c r="L16" s="43" t="n"/>
     </row>
     <row r="17" ht="14.4" customHeight="1">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="30" t="inlineStr">
+        <is>
+          <t>X1</t>
+        </is>
+      </c>
+      <c r="B17" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" s="30" t="n">
+        <v>40</v>
+      </c>
+      <c r="D17" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="44" t="n">
+        <v>50000000</v>
+      </c>
+      <c r="G17" s="44" t="n">
+        <v>40000000</v>
+      </c>
+      <c r="H17" s="44" t="n">
+        <v>2000000000</v>
+      </c>
+      <c r="I17" s="32" t="inlineStr">
+        <is>
+          <t>Quận 7</t>
+        </is>
+      </c>
+      <c r="J17" s="7" t="n"/>
+      <c r="K17" s="43" t="n"/>
+      <c r="L17" s="43" t="n"/>
+    </row>
+    <row r="18" ht="14.4" customHeight="1">
+      <c r="A18" s="30" t="inlineStr">
+        <is>
+          <t>X2</t>
+        </is>
+      </c>
+      <c r="B18" s="30" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" s="30" t="n">
+        <v>50</v>
+      </c>
+      <c r="D18" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="44" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="G18" s="44" t="n">
+        <v>50000000</v>
+      </c>
+      <c r="H18" s="44" t="n">
+        <v>4000000000</v>
+      </c>
+      <c r="I18" s="32" t="inlineStr">
+        <is>
+          <t>Quận 2</t>
+        </is>
+      </c>
+      <c r="J18" s="7" t="n"/>
+      <c r="K18" s="43" t="n"/>
+      <c r="L18" s="43" t="n"/>
+    </row>
+    <row r="19" ht="14.4" customHeight="1">
+      <c r="A19" t="inlineStr">
         <is>
           <t>x1</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="n">
-        <v>28</v>
-      </c>
-      <c r="D17" t="n">
+      <c r="B19" t="n">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>35</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="G19" t="n">
+        <v>50000000</v>
+      </c>
+      <c r="H19" t="n">
+        <v>3000000000</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Quận 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="14.4" customHeight="1">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>x2</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>30</v>
+      </c>
+      <c r="D20" t="n">
         <v>0</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E20" t="n">
         <v>0</v>
       </c>
-      <c r="F17" t="n">
-        <v>42000000</v>
-      </c>
-      <c r="G17" t="n">
-        <v>35000000</v>
-      </c>
-      <c r="H17" t="n">
-        <v>3500000000</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Quận 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="14.4" customHeight="1"/>
-    <row r="19" ht="14.4" customHeight="1"/>
-    <row r="20" ht="14.4" customHeight="1"/>
+      <c r="F20" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="G20" t="n">
+        <v>40000000</v>
+      </c>
+      <c r="H20" t="n">
+        <v>3000000000</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Quận 10</t>
+        </is>
+      </c>
+    </row>
     <row r="21" ht="14.4" customHeight="1"/>
     <row r="22" ht="14.4" customHeight="1"/>
     <row r="23" ht="14.4" customHeight="1"/>
@@ -30277,10 +30437,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -30339,17 +30499,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nghia Phan</t>
+          <t>Phan Nghĩa</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>phankhacbaonghia@gmail.com</t>
+          <t>test@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>test123@</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0365105521</t>
+          <t>0562612494</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -30357,9 +30522,41 @@
           <t>Bình Tân, Tp. Hồ Chí Minh</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>ACg8ocLZYigZHf2tSkEfIH0D1ZKUZT4DvPPj07pwIiz4VpIel3zXGTY=s96-c.jpg</t>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>x2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Nghĩa Phan</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>phannghia@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>phanghia123@</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0987654321</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Quận 9, Tp. Hồ Chí Minh</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Goku-Ultra-Instinct-PC-Wallpaper.jpg</t>
         </is>
       </c>
     </row>
@@ -30375,15 +30572,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="87.44140625" customWidth="1" min="1" max="1"/>
+    <col width="49.88671875" customWidth="1" min="3" max="3"/>
+    <col width="55.88671875" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="54" customHeight="1">
@@ -30392,6 +30591,52 @@
           <t>isValidInput(buyerInfo.get("group")) and isValidInput( buyerInfo.get("is_married")) and isValidInput( buyerInfo.get("no_child")) and isValidInput(houseInfo.get("no_bedroom"))</t>
         </is>
       </c>
+      <c r="C1" s="15" t="inlineStr">
+        <is>
+          <t>rule_expression</t>
+        </is>
+      </c>
+      <c r="G1" s="12" t="inlineStr">
+        <is>
+          <t>conditions</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="72" customHeight="1">
+      <c r="C2" s="16" t="inlineStr">
+        <is>
+          <t>(getValue(buyerInfo.get("group",  0))  == 1 or (buyerInfo.get("is_married")  == False and buyerInfo.get("no_child") == 0 )) and houseInfo.get("in_room_noBed")  in (1, 2)</t>
+        </is>
+      </c>
+      <c r="G2" s="12" t="inlineStr">
+        <is>
+          <t>isValidInput(buyerInfo.get("group")) and isValidInput( buyerInfo.get("is_married")) and isValidInput( buyerInfo.get("no_child")) and isValidInput(houseInfo.get("in_room_noBed"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="62.4" customHeight="1">
+      <c r="C3" s="16" t="inlineStr">
+        <is>
+          <t>(getValue(buyerInfo.get("group",  0))  == 1 or (buyerInfo.get("is_married")  == False and buyerInfo.get("no_child") == 0 )) and houseInfo.get("in_room_noBed")  in (2,3,4)</t>
+        </is>
+      </c>
+      <c r="G3" s="12" t="inlineStr">
+        <is>
+          <t>isNotNoneInput(buyerInfo.get("avai_amt")) and isNotNoneInput(buyerInfo.get("monthly_amt"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="62.4" customHeight="1">
+      <c r="C4" s="16" t="inlineStr">
+        <is>
+          <t>( getValue(buyerInfo.get("group",  0))  == 2 or buyerInfo.get("is_married")  == True ) and buyerInfo.get("no_child") in ( 0, 1) and houseInfo.get("in_room_noBed")  in (2, 3,4)</t>
+        </is>
+      </c>
+      <c r="G4" s="14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">isValidInput( buyerInfo.get("desired_location") ) and isValidInput( houseInfo.get("address_district") ) </t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="36" customHeight="1">
       <c r="A5" s="12" t="inlineStr">
@@ -30399,6 +30644,44 @@
           <t>isValidInput( buyerInfo.get("is_married")) and isValidInput( buyerInfo.get("no_child")) and isValidInput(houseInfo.get("no_bedroom"))</t>
         </is>
       </c>
+      <c r="C5" s="16" t="inlineStr">
+        <is>
+          <t>( getValue(buyerInfo.get("group",  0))  == 2 or buyerInfo.get("is_married")  == True ) and buyerInfo.get("no_child") in ( 0, 1) and houseInfo.get("in_room_noBed")  == 1</t>
+        </is>
+      </c>
+      <c r="G5" s="14" t="inlineStr">
+        <is>
+          <t>1==1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="62.4" customHeight="1">
+      <c r="C6" s="16" t="inlineStr">
+        <is>
+          <t>( getValue(buyerInfo.get("group",  0))  == 2 or buyerInfo.get("is_married")  == True ) and buyerInfo.get("no_child") == 2 and houseInfo.get("in_room_noBed")  == 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="62.4" customHeight="1">
+      <c r="C7" s="16" t="inlineStr">
+        <is>
+          <t>( getValue(buyerInfo.get("group",  0))  == 2 or buyerInfo.get("is_married")  == True )  and buyerInfo.get("no_child") == 2 and houseInfo.get("in_room_noBed")  in ( 3,4,5)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="31.2" customHeight="1">
+      <c r="C8" s="16" t="inlineStr">
+        <is>
+          <t>getValue(buyerInfo.get("group",  0))  == 4 and houseInfo.get("in_room_noBed")  == 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="31.2" customHeight="1">
+      <c r="C9" s="16" t="inlineStr">
+        <is>
+          <t>getValue(buyerInfo.get("group",  0))  == 4 and houseInfo.get("in_room_noBed")  in (2, 3,4)</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="36" customHeight="1">
       <c r="A10" s="12" t="inlineStr">
@@ -30406,11 +30689,91 @@
           <t>buyerInfo.get("avai_amt") is not None and buyerInfo.get("monthly_amt") is not None</t>
         </is>
       </c>
+      <c r="C10" s="17" t="inlineStr">
+        <is>
+          <t>houseInfo.get("price") &gt;= 0.9 * buyerInfo.get("avai_amt") and houseInfo.get("price") &lt;= buyerInfo.get("avai_amt")</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="93.59999999999999" customHeight="1">
+      <c r="C11" s="19" t="inlineStr">
+        <is>
+          <t>( buyerInfo.get("avai_amt")  &gt;= 0.75 * houseInfo.get("price") and houseInfo.get("price") &gt; buyerInfo.get("avai_amt") ) and ( (buyerInfo.get("avai_amt") + 12* buyerInfo.get("monthly_amt")) &gt;= houseInfo.get("price"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="93.59999999999999" customHeight="1">
+      <c r="C12" s="19" t="inlineStr">
+        <is>
+          <t>( buyerInfo.get("avai_amt")  &gt;= 0.5 * houseInfo.get("price") and houseInfo.get("price") &gt; buyerInfo.get("avai_amt") ) and ( (buyerInfo.get("avai_amt") + 24* buyerInfo.get("monthly_amt")) &gt;= houseInfo.get("price"))</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="54" customHeight="1">
       <c r="A13" s="12" t="inlineStr">
         <is>
           <t>isValidInput(buyerInfo.get("group")) and isValidInput( buyerInfo.get("is_married")) and isValidInput( buyerInfo.get("no_child")) and isValidInput(houseInfo.get("in_room_noBed"))</t>
+        </is>
+      </c>
+      <c r="C13" s="19" t="inlineStr">
+        <is>
+          <t>( buyerInfo.get("avai_amt")  &gt;= 0.5 * houseInfo.get("price") and houseInfo.get("price") &gt; buyerInfo.get("avai_amt") ) and ( (buyerInfo.get("avai_amt") + 60* buyerInfo.get("monthly_amt")) &gt;= houseInfo.get("price"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="62.4" customHeight="1">
+      <c r="C14" s="19" t="inlineStr">
+        <is>
+          <t>getValue(buyerInfo.get("group",  0))  == 4 and ( houseInfo.get("price") &gt;= 0.8 * buyerInfo.get("avai_amt") and houseInfo.get("price") &lt;= buyerInfo.get("avai_amt")*1.2 )</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="62.4" customHeight="1">
+      <c r="C15" s="19" t="inlineStr">
+        <is>
+          <t>getValue(buyerInfo.get("group",  0))  == 4 and ( houseInfo.get("price") &lt; 0.8 * buyerInfo.get("avai_amt") and houseInfo.get("price") &gt; buyerInfo.get("avai_amt")*1.2 )</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="31.2" customHeight="1">
+      <c r="C16" s="19" t="inlineStr">
+        <is>
+          <t>fn_calculateDistance(houseInfo.get("address_district"), buyerInfo.get("desired_location")) &lt;= 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="31.2" customHeight="1">
+      <c r="C17" s="19" t="inlineStr">
+        <is>
+          <t>fn_calculateDistance(houseInfo.get("address_district"), buyerInfo.get("desired_location")) &lt;= 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="31.2" customHeight="1">
+      <c r="C18" s="19" t="inlineStr">
+        <is>
+          <t>fn_calculateDistance(houseInfo.get("address_district"), buyerInfo.get("desired_location")) &lt;= 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="15.6" customHeight="1">
+      <c r="C19" s="19" t="inlineStr">
+        <is>
+          <t>isGoodLegalStatus(houseInfo.get("legal_status"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="46.8" customHeight="1">
+      <c r="C20" s="19" t="inlineStr">
+        <is>
+          <t>isGoodLegalStatus(houseInfo.get("legal_status")) is not True and getValue(buyerInfo.get("group",  0)) in (1, 3,4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="46.8" customHeight="1">
+      <c r="C21" s="19" t="inlineStr">
+        <is>
+          <t>isGoodLegalStatus(houseInfo.get("legal_status")) is not True and getValue(buyerInfo.get("group",  0)) not in (1, 3,4)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the comparison, added word and pptx
</commit_message>
<xml_diff>
--- a/model/data.xlsx
+++ b/model/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="658" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="658" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="rules" sheetId="1" state="visible" r:id="rId1"/>
@@ -186,7 +186,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -287,13 +287,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="11">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="9">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -686,15 +679,15 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
   <cols>
     <col width="13.33203125" customWidth="1" min="1" max="1"/>
     <col width="12.88671875" customWidth="1" min="2" max="2"/>
-    <col width="49.88671875" customWidth="1" style="39" min="4" max="4"/>
+    <col width="70.6640625" customWidth="1" style="39" min="4" max="4"/>
     <col width="55.44140625" customWidth="1" min="5" max="5"/>
     <col width="74" customWidth="1" min="6" max="6"/>
   </cols>
@@ -1001,7 +994,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="60.6" customHeight="1">
+    <row r="11" ht="73.8" customHeight="1">
       <c r="A11" s="18" t="inlineStr">
         <is>
           <t>B</t>
@@ -1027,7 +1020,7 @@
       </c>
       <c r="F11" s="20" t="n"/>
     </row>
-    <row r="12" ht="60.6" customHeight="1">
+    <row r="12" ht="78.59999999999999" customHeight="1">
       <c r="A12" s="18" t="inlineStr">
         <is>
           <t>B</t>
@@ -1057,7 +1050,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="60.6" customHeight="1">
+    <row r="13" ht="62.4" customHeight="1">
       <c r="A13" s="18" t="inlineStr">
         <is>
           <t>B</t>
@@ -1083,7 +1076,7 @@
       </c>
       <c r="F13" s="19" t="n"/>
     </row>
-    <row r="14" ht="60.6" customHeight="1">
+    <row r="14" ht="69" customHeight="1">
       <c r="A14" s="18" t="inlineStr">
         <is>
           <t>B</t>
@@ -1109,7 +1102,7 @@
       </c>
       <c r="F14" s="19" t="n"/>
     </row>
-    <row r="15" ht="60.6" customHeight="1">
+    <row r="15" ht="72.59999999999999" customHeight="1">
       <c r="A15" s="18" t="inlineStr">
         <is>
           <t>B</t>
@@ -1301,7 +1294,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1356,7 +1349,7 @@
       </c>
       <c r="B2" s="40" t="inlineStr">
         <is>
-          <t>isValidInput( buyerInfo.get("group") )  and isValidInput( buyerInfo.get("is_married") )  and isValidInput( buyerInfo.get("no_child") )  and isValidInput(houseInfo.get("no_bedroom") )</t>
+          <t>isValidInput( buyerInfo.get("group") )  and isValidInput( buyerInfo.get("is_married") )  and isValidInput( buyerInfo.get("no_child") )  and isValidInput(houseInfo.get("in_room_noBed") )</t>
         </is>
       </c>
       <c r="C2" s="12" t="n"/>
@@ -1483,26 +1476,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col width="3.5546875" bestFit="1" customWidth="1" style="43" min="1" max="1"/>
-    <col width="7.33203125" customWidth="1" style="43" min="2" max="2"/>
-    <col width="8.88671875" customWidth="1" style="43" min="3" max="3"/>
-    <col width="11.33203125" bestFit="1" customWidth="1" style="43" min="4" max="4"/>
-    <col width="9.6640625" customWidth="1" style="43" min="5" max="5"/>
+    <col width="3.5546875" bestFit="1" customWidth="1" style="22" min="1" max="1"/>
+    <col width="7.33203125" customWidth="1" style="22" min="2" max="2"/>
+    <col width="8.88671875" customWidth="1" style="22" min="3" max="3"/>
+    <col width="11.33203125" bestFit="1" customWidth="1" style="22" min="4" max="4"/>
+    <col width="9.6640625" customWidth="1" style="22" min="5" max="5"/>
     <col width="15.33203125" customWidth="1" style="28" min="6" max="6"/>
     <col width="15.77734375" customWidth="1" style="28" min="7" max="7"/>
     <col width="18.109375" bestFit="1" customWidth="1" style="28" min="8" max="8"/>
-    <col width="18.21875" customWidth="1" style="43" min="9" max="9"/>
-    <col width="22.88671875" bestFit="1" customWidth="1" style="43" min="10" max="10"/>
-    <col width="8.88671875" customWidth="1" style="43" min="11" max="43"/>
-    <col width="8.88671875" customWidth="1" style="43" min="44" max="16384"/>
+    <col width="18.21875" customWidth="1" style="22" min="9" max="9"/>
+    <col width="22.88671875" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
+    <col width="8.88671875" customWidth="1" style="22" min="11" max="45"/>
+    <col width="8.88671875" customWidth="1" style="22" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1556,7 +1549,7 @@
           <t>desired_interiorStatus</t>
         </is>
       </c>
-      <c r="K1" s="42" t="n"/>
+      <c r="K1" s="8" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
@@ -1591,7 +1584,7 @@
         </is>
       </c>
       <c r="J2" s="7" t="n"/>
-      <c r="K2" s="42" t="n"/>
+      <c r="K2" s="8" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
@@ -1626,7 +1619,7 @@
         </is>
       </c>
       <c r="J3" s="7" t="n"/>
-      <c r="K3" s="42" t="n"/>
+      <c r="K3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
@@ -1661,7 +1654,7 @@
         </is>
       </c>
       <c r="J4" s="7" t="n"/>
-      <c r="K4" s="42" t="n"/>
+      <c r="K4" s="8" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
@@ -1696,7 +1689,7 @@
         </is>
       </c>
       <c r="J5" s="7" t="n"/>
-      <c r="K5" s="42" t="n"/>
+      <c r="K5" s="8" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
@@ -1721,7 +1714,7 @@
       <c r="H6" s="26" t="n"/>
       <c r="I6" s="7" t="n"/>
       <c r="J6" s="7" t="n"/>
-      <c r="K6" s="42" t="n"/>
+      <c r="K6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
@@ -1915,7 +1908,7 @@
         </is>
       </c>
       <c r="J14" s="7" t="n"/>
-      <c r="K14" s="42" t="n"/>
+      <c r="K14" s="8" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="7" t="inlineStr">
@@ -1936,8 +1929,7 @@
         </is>
       </c>
       <c r="J15" s="7" t="n"/>
-      <c r="K15" s="42" t="n"/>
-      <c r="L15" s="43" t="n"/>
+      <c r="K15" s="8" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="33" t="inlineStr">
@@ -1956,8 +1948,7 @@
       <c r="H16" s="34" t="n"/>
       <c r="I16" s="33" t="n"/>
       <c r="J16" s="33" t="n"/>
-      <c r="K16" s="42" t="n"/>
-      <c r="L16" s="43" t="n"/>
+      <c r="K16" s="8" t="n"/>
     </row>
     <row r="17" ht="14.4" customHeight="1">
       <c r="A17" s="30" t="inlineStr">
@@ -1977,13 +1968,13 @@
       <c r="E17" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="44" t="n">
+      <c r="F17" s="31" t="n">
         <v>50000000</v>
       </c>
-      <c r="G17" s="44" t="n">
+      <c r="G17" s="31" t="n">
         <v>40000000</v>
       </c>
-      <c r="H17" s="44" t="n">
+      <c r="H17" s="31" t="n">
         <v>2000000000</v>
       </c>
       <c r="I17" s="32" t="inlineStr">
@@ -1992,8 +1983,6 @@
         </is>
       </c>
       <c r="J17" s="7" t="n"/>
-      <c r="K17" s="43" t="n"/>
-      <c r="L17" s="43" t="n"/>
     </row>
     <row r="18" ht="14.4" customHeight="1">
       <c r="A18" s="30" t="inlineStr">
@@ -2013,13 +2002,13 @@
       <c r="E18" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="F18" s="44" t="n">
+      <c r="F18" s="31" t="n">
         <v>30000000</v>
       </c>
-      <c r="G18" s="44" t="n">
+      <c r="G18" s="31" t="n">
         <v>50000000</v>
       </c>
-      <c r="H18" s="44" t="n">
+      <c r="H18" s="31" t="n">
         <v>4000000000</v>
       </c>
       <c r="I18" s="32" t="inlineStr">
@@ -2028,8 +2017,6 @@
         </is>
       </c>
       <c r="J18" s="7" t="n"/>
-      <c r="K18" s="43" t="n"/>
-      <c r="L18" s="43" t="n"/>
     </row>
     <row r="19" ht="14.4" customHeight="1">
       <c r="A19" t="inlineStr">
@@ -2038,10 +2025,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C19" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
@@ -2056,11 +2043,11 @@
         <v>50000000</v>
       </c>
       <c r="H19" t="n">
-        <v>3000000000</v>
+        <v>20000000000</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Quận 10</t>
+          <t>Thủ Đức</t>
         </is>
       </c>
     </row>
@@ -2083,21 +2070,53 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>30000000</v>
+        <v>70000000</v>
       </c>
       <c r="G20" t="n">
-        <v>40000000</v>
+        <v>50000000</v>
       </c>
       <c r="H20" t="n">
-        <v>3000000000</v>
+        <v>10000000000</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Quận 10</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="14.4" customHeight="1"/>
+          <t>Quận 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="14.4" customHeight="1">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>x3</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" t="n">
+        <v>40</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" t="n">
+        <v>300000000</v>
+      </c>
+      <c r="G21" t="n">
+        <v>250000000</v>
+      </c>
+      <c r="H21" t="n">
+        <v>6000000000</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Quận 1</t>
+        </is>
+      </c>
+    </row>
     <row r="22" ht="14.4" customHeight="1"/>
     <row r="23" ht="14.4" customHeight="1"/>
   </sheetData>
@@ -30437,7 +30456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
@@ -30541,7 +30560,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>phanghia123@</t>
+          <t>phannghia123@</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -30557,6 +30576,38 @@
       <c r="G3" t="inlineStr">
         <is>
           <t>Goku-Ultra-Instinct-PC-Wallpaper.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>x3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Phan Nghia</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>test123@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>test123@</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0334562766</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1159 tinh lo 10, Tan Tao</t>
         </is>
       </c>
     </row>

</xml_diff>